<commit_message>
Clean up old files; add UseCaseContainer
</commit_message>
<xml_diff>
--- a/project/excel/standards_schema_all.xlsx
+++ b/project/excel/standards_schema_all.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="29" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="31" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="BiomedicalStandard" sheetId="1" state="visible" r:id="rId1"/>
@@ -22,21 +22,23 @@
     <sheet name="SoftwareOrTool" sheetId="13" state="visible" r:id="rId13"/>
     <sheet name="TrainingProgram" sheetId="14" state="visible" r:id="rId14"/>
     <sheet name="UseCase" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="BiomedicalStandard1" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="DataStandard1" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="DataStandardOrTool1" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="DataSubstrate1" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="DataTopic1" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet name="ModelRepository1" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="NamedThing1" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet name="OntologyOrVocabulary1" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet name="Organization1" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet name="ReferenceDataOrDataset1" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet name="ReferenceImplementation1" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet name="Registry1" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet name="SoftwareOrTool1" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet name="TrainingProgram1" sheetId="29" state="visible" r:id="rId29"/>
-    <sheet name="UseCase1" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="UseCaseContainer" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="BiomedicalStandard1" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="DataStandard1" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="DataStandardOrTool1" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="DataSubstrate1" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="DataTopic1" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="ModelRepository1" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="NamedThing1" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="OntologyOrVocabulary1" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="Organization1" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="ReferenceDataOrDataset1" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="ReferenceImplementation1" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="Registry1" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="SoftwareOrTool1" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="TrainingProgram1" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="UseCase1" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="UseCaseContainer1" sheetId="32" state="visible" r:id="rId32"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1059,7 +1061,7 @@
     <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>"acquisition,integration,standardization,modeling,application,assessment"</formula1>
     </dataValidation>
-    <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>"aireadi,chorus,cm4ai,voice"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1073,6 +1075,37 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>container_name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>use_cases</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1153,7 +1186,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1239,7 +1272,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1325,7 +1358,93 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:M1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>subclass_of</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>collection</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>concerns_data_topic</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>has_relevant_organization</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>purpose_detail</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>is_open</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>requires_registration</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>url</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>publication</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>formal_specification</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1396,7 +1515,63 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>subclass_of</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>EDAM_ID</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>MeSH_ID</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>NCIT_ID</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1482,13 +1657,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1517,34 +1692,105 @@
           <t>subclass_of</t>
         </is>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:M1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>subclass_of</t>
+        </is>
+      </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>EDAM_ID</t>
+          <t>collection</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>MeSH_ID</t>
+          <t>concerns_data_topic</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>NCIT_ID</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:M1"/>
+          <t>has_relevant_organization</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>purpose_detail</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>is_open</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>requires_registration</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>url</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>publication</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>formal_specification</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1575,321 +1821,22 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>collection</t>
+          <t>ROR_ID</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>concerns_data_topic</t>
+          <t>Wikidata_ID</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>has_relevant_organization</t>
+          <t>URL</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>purpose_detail</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>is_open</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>requires_registration</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>url</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>publication</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>formal_specification</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>subclass_of</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:M1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>subclass_of</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>collection</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>concerns_data_topic</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>has_relevant_organization</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>purpose_detail</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>is_open</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>requires_registration</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>url</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>publication</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>formal_specification</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>subclass_of</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>ROR_ID</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Wikidata_ID</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>URL</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
           <t>related_to</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:M1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>subclass_of</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>collection</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>concerns_data_topic</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>has_relevant_organization</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>purpose_detail</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>is_open</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>requires_registration</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>url</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>publication</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>formal_specification</t>
         </is>
       </c>
     </row>
@@ -2342,6 +2289,92 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:M1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>subclass_of</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>collection</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>concerns_data_topic</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>has_relevant_organization</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>purpose_detail</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>is_open</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>requires_registration</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>url</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>publication</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>formal_specification</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:P1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2437,6 +2470,37 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>container_name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>use_cases</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
Add OrganizationContainer; restructure UseCase; remove container_name
</commit_message>
<xml_diff>
--- a/project/excel/standards_schema_all.xlsx
+++ b/project/excel/standards_schema_all.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="31" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="33" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="BiomedicalStandard" sheetId="1" state="visible" r:id="rId1"/>
@@ -16,29 +16,31 @@
     <sheet name="NamedThing" sheetId="7" state="visible" r:id="rId7"/>
     <sheet name="OntologyOrVocabulary" sheetId="8" state="visible" r:id="rId8"/>
     <sheet name="Organization" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="ReferenceDataOrDataset" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="ReferenceImplementation" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="Registry" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="SoftwareOrTool" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="TrainingProgram" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="UseCase" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="UseCaseContainer" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="BiomedicalStandard1" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="DataStandard1" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="DataStandardOrTool1" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="DataSubstrate1" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet name="DataTopic1" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="ModelRepository1" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet name="NamedThing1" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet name="OntologyOrVocabulary1" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet name="Organization1" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet name="ReferenceDataOrDataset1" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet name="ReferenceImplementation1" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet name="Registry1" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet name="SoftwareOrTool1" sheetId="29" state="visible" r:id="rId29"/>
-    <sheet name="TrainingProgram1" sheetId="30" state="visible" r:id="rId30"/>
-    <sheet name="UseCase1" sheetId="31" state="visible" r:id="rId31"/>
-    <sheet name="UseCaseContainer1" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="OrganizationContainer" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="ReferenceDataOrDataset" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="ReferenceImplementation" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="Registry" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="SoftwareOrTool" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="TrainingProgram" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="UseCase" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="UseCaseContainer" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="BiomedicalStandard1" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="DataStandard1" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="DataStandardOrTool1" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="DataSubstrate1" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="DataTopic1" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="ModelRepository1" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="NamedThing1" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="OntologyOrVocabulary1" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="Organization1" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="OrganizationContainer1" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="ReferenceDataOrDataset1" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="ReferenceImplementation1" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="Registry1" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="SoftwareOrTool1" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="TrainingProgram1" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="UseCase1" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="UseCaseContainer1" sheetId="34" state="visible" r:id="rId34"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -530,6 +532,32 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>organizations</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -610,7 +638,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -696,7 +724,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -782,7 +810,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -868,7 +896,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -954,7 +982,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1069,38 +1097,119 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>container_name</t>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>use_cases</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:M1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>use_cases</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>subclass_of</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>collection</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>concerns_data_topic</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>has_relevant_organization</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>purpose_detail</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>is_open</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>requires_registration</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>url</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>publication</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>formal_specification</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1186,7 +1295,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1272,7 +1381,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1358,7 +1467,134 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>subclass_of</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>EDAM_ID</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>MeSH_ID</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>NCIT_ID</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>metadata_storage</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>file_extensions</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>limitations</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>subclass_of</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>EDAM_ID</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>MeSH_ID</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>NCIT_ID</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1444,13 +1680,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J1"/>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1479,49 +1715,105 @@
           <t>subclass_of</t>
         </is>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:M1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>subclass_of</t>
+        </is>
+      </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>EDAM_ID</t>
+          <t>collection</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>MeSH_ID</t>
+          <t>concerns_data_topic</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>NCIT_ID</t>
+          <t>has_relevant_organization</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>metadata_storage</t>
+          <t>purpose_detail</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>file_extensions</t>
+          <t>is_open</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>limitations</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
+          <t>requires_registration</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>url</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>publication</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>formal_specification</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1552,290 +1844,21 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>EDAM_ID</t>
+          <t>ROR_ID</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>MeSH_ID</t>
+          <t>Wikidata_ID</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>NCIT_ID</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:M1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>subclass_of</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>collection</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>concerns_data_topic</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>has_relevant_organization</t>
+          <t>URL</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>purpose_detail</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>is_open</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>requires_registration</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>url</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>publication</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>formal_specification</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>subclass_of</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:M1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>subclass_of</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>collection</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>concerns_data_topic</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>has_relevant_organization</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>purpose_detail</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>is_open</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>requires_registration</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>url</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>publication</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>formal_specification</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>subclass_of</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>ROR_ID</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Wikidata_ID</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>URL</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
           <t>related_to</t>
         </is>
       </c>
@@ -1845,170 +1868,24 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:M1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>subclass_of</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>collection</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>concerns_data_topic</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>has_relevant_organization</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>purpose_detail</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>is_open</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>requires_registration</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>url</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>publication</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>formal_specification</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>subclass_of</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>collection</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>concerns_data_topic</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>has_relevant_organization</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>purpose_detail</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>is_open</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>requires_registration</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>url</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>publication</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>formal_specification</t>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>organizations</t>
         </is>
       </c>
     </row>
@@ -2375,6 +2252,178 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:M1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>subclass_of</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>collection</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>concerns_data_topic</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>has_relevant_organization</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>purpose_detail</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>is_open</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>requires_registration</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>url</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>publication</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>formal_specification</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:M1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>subclass_of</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>collection</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>concerns_data_topic</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>has_relevant_organization</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>purpose_detail</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>is_open</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>requires_registration</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>url</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>publication</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>formal_specification</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:P1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2470,44 +2519,110 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>container_name</t>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>use_cases</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>use_cases</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J1"/>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>subclass_of</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>EDAM_ID</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>MeSH_ID</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>NCIT_ID</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>metadata_storage</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>file_extensions</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>limitations</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2551,34 +2666,105 @@
           <t>NCIT_ID</t>
         </is>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:M1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>subclass_of</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>collection</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>concerns_data_topic</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>has_relevant_organization</t>
+        </is>
+      </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>metadata_storage</t>
+          <t>purpose_detail</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>file_extensions</t>
+          <t>is_open</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>limitations</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
+          <t>requires_registration</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>url</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>publication</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>formal_specification</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2607,34 +2793,105 @@
           <t>subclass_of</t>
         </is>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:M1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>subclass_of</t>
+        </is>
+      </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>EDAM_ID</t>
+          <t>collection</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>MeSH_ID</t>
+          <t>concerns_data_topic</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>NCIT_ID</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:M1"/>
+          <t>has_relevant_organization</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>purpose_detail</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>is_open</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>requires_registration</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>url</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>publication</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>formal_specification</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2665,234 +2922,21 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>collection</t>
+          <t>ROR_ID</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>concerns_data_topic</t>
+          <t>Wikidata_ID</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>has_relevant_organization</t>
+          <t>URL</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>purpose_detail</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>is_open</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>requires_registration</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>url</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>publication</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>formal_specification</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>subclass_of</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:M1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>subclass_of</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>collection</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>concerns_data_topic</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>has_relevant_organization</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>purpose_detail</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>is_open</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>requires_registration</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>url</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>publication</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>formal_specification</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>subclass_of</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>ROR_ID</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Wikidata_ID</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>URL</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
           <t>related_to</t>
         </is>
       </c>

</xml_diff>

<commit_message>
Add valid examples; artifacts; repair metadata_storage slot range
</commit_message>
<xml_diff>
--- a/project/excel/standards_schema_all.xlsx
+++ b/project/excel/standards_schema_all.xlsx
@@ -696,17 +696,17 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>ROR_ID</t>
+          <t>ror_id</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>Wikidata_ID</t>
+          <t>wikidata_id</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>URL</t>
+          <t>url</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
@@ -1724,17 +1724,17 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>EDAM_ID</t>
+          <t>edam_id</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>MeSH_ID</t>
+          <t>mesh_id</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>NCIT_ID</t>
+          <t>ncit_id</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
@@ -1821,17 +1821,17 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>EDAM_ID</t>
+          <t>edam_id</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>MeSH_ID</t>
+          <t>mesh_id</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>NCIT_ID</t>
+          <t>ncit_id</t>
         </is>
       </c>
     </row>
@@ -2210,17 +2210,17 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>ROR_ID</t>
+          <t>ror_id</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>Wikidata_ID</t>
+          <t>wikidata_id</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>URL</t>
+          <t>url</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
@@ -2880,17 +2880,17 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>EDAM_ID</t>
+          <t>edam_id</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>MeSH_ID</t>
+          <t>mesh_id</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>NCIT_ID</t>
+          <t>ncit_id</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
@@ -2977,17 +2977,17 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>EDAM_ID</t>
+          <t>edam_id</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>MeSH_ID</t>
+          <t>mesh_id</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>NCIT_ID</t>
+          <t>ncit_id</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update project artifacts and docs
</commit_message>
<xml_diff>
--- a/project/excel/standards_schema_all.xlsx
+++ b/project/excel/standards_schema_all.xlsx
@@ -23,10 +23,11 @@
     <sheet name="DataTopic" sheetId="14" state="visible" r:id="rId14"/>
     <sheet name="DataTopicContainer" sheetId="15" state="visible" r:id="rId15"/>
     <sheet name="NamedThing" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="Organization" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="OrganizationContainer" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="DataSubstrate" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="DataSubstrateContainer" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="AnatomicalEntity" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="Organization" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="OrganizationContainer" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="DataSubstrate" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="DataSubstrateContainer" sheetId="21" state="visible" r:id="rId21"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1158,6 +1159,77 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>category</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>subclass_of</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>related_to</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>contributor_name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>contributor_github_name</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>contributor_orcid</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>contribution_date</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1238,7 +1310,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1256,107 +1328,6 @@
       <c r="A1" t="inlineStr">
         <is>
           <t>organizations</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:P1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>edam_id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>mesh_id</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>ncit_id</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>metadata_storage</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>file_extensions</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>limitations</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>category</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>subclass_of</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>related_to</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>contributor_name</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>contributor_github_name</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>contributor_orcid</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>contribution_date</t>
         </is>
       </c>
     </row>
@@ -1392,6 +1363,107 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:P1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>edam_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>mesh_id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>ncit_id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>metadata_storage</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>file_extensions</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>limitations</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>category</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>subclass_of</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>related_to</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>contributor_name</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>contributor_github_name</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>contributor_orcid</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>contribution_date</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>

<commit_message>
Add slot properly; update artifacts; add new example
</commit_message>
<xml_diff>
--- a/project/excel/standards_schema_all.xlsx
+++ b/project/excel/standards_schema_all.xlsx
@@ -976,7 +976,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1002,50 +1002,55 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>topic_involves_anatomy</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>category</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>subclass_of</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>related_to</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>contributor_name</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>contributor_github_name</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>contributor_orcid</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>contribution_date</t>
         </is>

</xml_diff>

<commit_message>
Add has_ai_application to StandardsCollectionTag; update project artifacts
</commit_message>
<xml_diff>
--- a/project/excel/standards_schema_all.xlsx
+++ b/project/excel/standards_schema_all.xlsx
@@ -685,7 +685,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"audiovisual,deprecated,fileformat,toolkit,clinicaldata,multimodal,text,cloudplatform,cloudservice,codesystem,datamodel,dataregistry,softwareregistry,datavisualization,notebookplatform,datasheets,machinelearningframework,workflowlanguage,diagnosticinstrument,drugdata,eyedata,markuplanguage,graphdataplatform,guidelines,minimuminformationschema,modelcards,obofoundry,ontologyregistry,policy,proteindata,referencegenome,scrnaseqanalysis,speechdata,standardsregistry"</formula1>
+      <formula1>"audiovisual,deprecated,fileformat,toolkit,clinicaldata,multimodal,text,cloudplatform,cloudservice,codesystem,datamodel,dataregistry,softwareregistry,datavisualization,notebookplatform,datasheets,machinelearningframework,workflowlanguage,diagnosticinstrument,drugdata,eyedata,markuplanguage,graphdataplatform,guidelines,minimuminformationschema,modelcards,obofoundry,ontologyregistry,policy,proteindata,referencegenome,scrnaseqanalysis,speechdata,standardsregistry,has_ai_application"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -811,7 +811,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"audiovisual,deprecated,fileformat,toolkit,clinicaldata,multimodal,text,cloudplatform,cloudservice,codesystem,datamodel,dataregistry,softwareregistry,datavisualization,notebookplatform,datasheets,machinelearningframework,workflowlanguage,diagnosticinstrument,drugdata,eyedata,markuplanguage,graphdataplatform,guidelines,minimuminformationschema,modelcards,obofoundry,ontologyregistry,policy,proteindata,referencegenome,scrnaseqanalysis,speechdata,standardsregistry"</formula1>
+      <formula1>"audiovisual,deprecated,fileformat,toolkit,clinicaldata,multimodal,text,cloudplatform,cloudservice,codesystem,datamodel,dataregistry,softwareregistry,datavisualization,notebookplatform,datasheets,machinelearningframework,workflowlanguage,diagnosticinstrument,drugdata,eyedata,markuplanguage,graphdataplatform,guidelines,minimuminformationschema,modelcards,obofoundry,ontologyregistry,policy,proteindata,referencegenome,scrnaseqanalysis,speechdata,standardsregistry,has_ai_application"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -937,7 +937,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"audiovisual,deprecated,fileformat,toolkit,clinicaldata,multimodal,text,cloudplatform,cloudservice,codesystem,datamodel,dataregistry,softwareregistry,datavisualization,notebookplatform,datasheets,machinelearningframework,workflowlanguage,diagnosticinstrument,drugdata,eyedata,markuplanguage,graphdataplatform,guidelines,minimuminformationschema,modelcards,obofoundry,ontologyregistry,policy,proteindata,referencegenome,scrnaseqanalysis,speechdata,standardsregistry"</formula1>
+      <formula1>"audiovisual,deprecated,fileformat,toolkit,clinicaldata,multimodal,text,cloudplatform,cloudservice,codesystem,datamodel,dataregistry,softwareregistry,datavisualization,notebookplatform,datasheets,machinelearningframework,workflowlanguage,diagnosticinstrument,drugdata,eyedata,markuplanguage,graphdataplatform,guidelines,minimuminformationschema,modelcards,obofoundry,ontologyregistry,policy,proteindata,referencegenome,scrnaseqanalysis,speechdata,standardsregistry,has_ai_application"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1613,7 +1613,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"audiovisual,deprecated,fileformat,toolkit,clinicaldata,multimodal,text,cloudplatform,cloudservice,codesystem,datamodel,dataregistry,softwareregistry,datavisualization,notebookplatform,datasheets,machinelearningframework,workflowlanguage,diagnosticinstrument,drugdata,eyedata,markuplanguage,graphdataplatform,guidelines,minimuminformationschema,modelcards,obofoundry,ontologyregistry,policy,proteindata,referencegenome,scrnaseqanalysis,speechdata,standardsregistry"</formula1>
+      <formula1>"audiovisual,deprecated,fileformat,toolkit,clinicaldata,multimodal,text,cloudplatform,cloudservice,codesystem,datamodel,dataregistry,softwareregistry,datavisualization,notebookplatform,datasheets,machinelearningframework,workflowlanguage,diagnosticinstrument,drugdata,eyedata,markuplanguage,graphdataplatform,guidelines,minimuminformationschema,modelcards,obofoundry,ontologyregistry,policy,proteindata,referencegenome,scrnaseqanalysis,speechdata,standardsregistry,has_ai_application"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1739,7 +1739,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"audiovisual,deprecated,fileformat,toolkit,clinicaldata,multimodal,text,cloudplatform,cloudservice,codesystem,datamodel,dataregistry,softwareregistry,datavisualization,notebookplatform,datasheets,machinelearningframework,workflowlanguage,diagnosticinstrument,drugdata,eyedata,markuplanguage,graphdataplatform,guidelines,minimuminformationschema,modelcards,obofoundry,ontologyregistry,policy,proteindata,referencegenome,scrnaseqanalysis,speechdata,standardsregistry"</formula1>
+      <formula1>"audiovisual,deprecated,fileformat,toolkit,clinicaldata,multimodal,text,cloudplatform,cloudservice,codesystem,datamodel,dataregistry,softwareregistry,datavisualization,notebookplatform,datasheets,machinelearningframework,workflowlanguage,diagnosticinstrument,drugdata,eyedata,markuplanguage,graphdataplatform,guidelines,minimuminformationschema,modelcards,obofoundry,ontologyregistry,policy,proteindata,referencegenome,scrnaseqanalysis,speechdata,standardsregistry,has_ai_application"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1865,7 +1865,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"audiovisual,deprecated,fileformat,toolkit,clinicaldata,multimodal,text,cloudplatform,cloudservice,codesystem,datamodel,dataregistry,softwareregistry,datavisualization,notebookplatform,datasheets,machinelearningframework,workflowlanguage,diagnosticinstrument,drugdata,eyedata,markuplanguage,graphdataplatform,guidelines,minimuminformationschema,modelcards,obofoundry,ontologyregistry,policy,proteindata,referencegenome,scrnaseqanalysis,speechdata,standardsregistry"</formula1>
+      <formula1>"audiovisual,deprecated,fileformat,toolkit,clinicaldata,multimodal,text,cloudplatform,cloudservice,codesystem,datamodel,dataregistry,softwareregistry,datavisualization,notebookplatform,datasheets,machinelearningframework,workflowlanguage,diagnosticinstrument,drugdata,eyedata,markuplanguage,graphdataplatform,guidelines,minimuminformationschema,modelcards,obofoundry,ontologyregistry,policy,proteindata,referencegenome,scrnaseqanalysis,speechdata,standardsregistry,has_ai_application"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1991,7 +1991,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"audiovisual,deprecated,fileformat,toolkit,clinicaldata,multimodal,text,cloudplatform,cloudservice,codesystem,datamodel,dataregistry,softwareregistry,datavisualization,notebookplatform,datasheets,machinelearningframework,workflowlanguage,diagnosticinstrument,drugdata,eyedata,markuplanguage,graphdataplatform,guidelines,minimuminformationschema,modelcards,obofoundry,ontologyregistry,policy,proteindata,referencegenome,scrnaseqanalysis,speechdata,standardsregistry"</formula1>
+      <formula1>"audiovisual,deprecated,fileformat,toolkit,clinicaldata,multimodal,text,cloudplatform,cloudservice,codesystem,datamodel,dataregistry,softwareregistry,datavisualization,notebookplatform,datasheets,machinelearningframework,workflowlanguage,diagnosticinstrument,drugdata,eyedata,markuplanguage,graphdataplatform,guidelines,minimuminformationschema,modelcards,obofoundry,ontologyregistry,policy,proteindata,referencegenome,scrnaseqanalysis,speechdata,standardsregistry,has_ai_application"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2117,7 +2117,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"audiovisual,deprecated,fileformat,toolkit,clinicaldata,multimodal,text,cloudplatform,cloudservice,codesystem,datamodel,dataregistry,softwareregistry,datavisualization,notebookplatform,datasheets,machinelearningframework,workflowlanguage,diagnosticinstrument,drugdata,eyedata,markuplanguage,graphdataplatform,guidelines,minimuminformationschema,modelcards,obofoundry,ontologyregistry,policy,proteindata,referencegenome,scrnaseqanalysis,speechdata,standardsregistry"</formula1>
+      <formula1>"audiovisual,deprecated,fileformat,toolkit,clinicaldata,multimodal,text,cloudplatform,cloudservice,codesystem,datamodel,dataregistry,softwareregistry,datavisualization,notebookplatform,datasheets,machinelearningframework,workflowlanguage,diagnosticinstrument,drugdata,eyedata,markuplanguage,graphdataplatform,guidelines,minimuminformationschema,modelcards,obofoundry,ontologyregistry,policy,proteindata,referencegenome,scrnaseqanalysis,speechdata,standardsregistry,has_ai_application"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2243,7 +2243,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"audiovisual,deprecated,fileformat,toolkit,clinicaldata,multimodal,text,cloudplatform,cloudservice,codesystem,datamodel,dataregistry,softwareregistry,datavisualization,notebookplatform,datasheets,machinelearningframework,workflowlanguage,diagnosticinstrument,drugdata,eyedata,markuplanguage,graphdataplatform,guidelines,minimuminformationschema,modelcards,obofoundry,ontologyregistry,policy,proteindata,referencegenome,scrnaseqanalysis,speechdata,standardsregistry"</formula1>
+      <formula1>"audiovisual,deprecated,fileformat,toolkit,clinicaldata,multimodal,text,cloudplatform,cloudservice,codesystem,datamodel,dataregistry,softwareregistry,datavisualization,notebookplatform,datasheets,machinelearningframework,workflowlanguage,diagnosticinstrument,drugdata,eyedata,markuplanguage,graphdataplatform,guidelines,minimuminformationschema,modelcards,obofoundry,ontologyregistry,policy,proteindata,referencegenome,scrnaseqanalysis,speechdata,standardsregistry,has_ai_application"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2369,7 +2369,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"audiovisual,deprecated,fileformat,toolkit,clinicaldata,multimodal,text,cloudplatform,cloudservice,codesystem,datamodel,dataregistry,softwareregistry,datavisualization,notebookplatform,datasheets,machinelearningframework,workflowlanguage,diagnosticinstrument,drugdata,eyedata,markuplanguage,graphdataplatform,guidelines,minimuminformationschema,modelcards,obofoundry,ontologyregistry,policy,proteindata,referencegenome,scrnaseqanalysis,speechdata,standardsregistry"</formula1>
+      <formula1>"audiovisual,deprecated,fileformat,toolkit,clinicaldata,multimodal,text,cloudplatform,cloudservice,codesystem,datamodel,dataregistry,softwareregistry,datavisualization,notebookplatform,datasheets,machinelearningframework,workflowlanguage,diagnosticinstrument,drugdata,eyedata,markuplanguage,graphdataplatform,guidelines,minimuminformationschema,modelcards,obofoundry,ontologyregistry,policy,proteindata,referencegenome,scrnaseqanalysis,speechdata,standardsregistry,has_ai_application"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>